<commit_message>
(#232)disabled failing cts tests - removed bad data from excel data providers - modified test data sets - modified status code test data - updated POM
</commit_message>
<xml_diff>
--- a/test-data/bread-crumb-data.xlsx
+++ b/test-data/bread-crumb-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashkinaea/IdeaProjects/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C19D25A-42C1-48F8-B107-E925D5364FEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2796A04-6A37-3E4C-B763-DC7AEC253C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_breadcrumbs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>path</t>
   </si>
@@ -99,12 +99,6 @@
     <t>Cancer Type Homepage</t>
   </si>
   <si>
-    <t>Mini Landing Page</t>
-  </si>
-  <si>
-    <t>about-nci/organization/dcb/division-of-cancer-biology-test</t>
-  </si>
-  <si>
     <t>types/breast/research</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>types/stomach/patient/stomach-treatment-pdq</t>
   </si>
   <si>
-    <t>news-events/press-releases/2019/brca-exchange-test</t>
-  </si>
-  <si>
     <t>Press Release</t>
   </si>
   <si>
@@ -214,12 +205,6 @@
   </si>
   <si>
     <t>Página principal,Noticias</t>
-  </si>
-  <si>
-    <t>Home,About NCI,NCI Organization</t>
-  </si>
-  <si>
-    <t>/,/about-nci,/about-nci/organization</t>
   </si>
   <si>
     <t>Home,About Cancer,Coping with Cancer,Feelings and Cancer,Learning to Relax</t>
@@ -587,21 +572,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E50E58-C20E-6840-B475-2B9A8D9E132C}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.875" customWidth="1"/>
-    <col min="4" max="4" width="51.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.375" customWidth="1"/>
+    <col min="1" max="1" width="70.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -612,13 +597,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -629,15 +614,15 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -646,13 +631,13 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -663,30 +648,30 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -697,15 +682,15 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -714,13 +699,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -731,13 +716,13 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -748,13 +733,13 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -765,13 +750,13 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -782,13 +767,13 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -799,13 +784,13 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -816,112 +801,78 @@
         <v>17</v>
       </c>
       <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -933,17 +884,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D54F65-9878-4854-8CCD-A6423ADC111E}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.875" customWidth="1"/>
-    <col min="2" max="2" width="24.875" customWidth="1"/>
+    <col min="1" max="1" width="44.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -954,23 +905,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>